<commit_message>
Replacing K9HZ amplifier with updated AC8GY design, at the request of K9HZ.
</commit_message>
<xml_diff>
--- a/pcbs/20w_pa/manufacturing/SMD_BOM.xlsx
+++ b/pcbs/20w_pa/manufacturing/SMD_BOM.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="109">
   <si>
     <t xml:space="preserve">xxxx xxxx xxxxx xxPCS BOM  (Sample Bill of Materials)</t>
   </si>
@@ -134,211 +134,295 @@
     <t xml:space="preserve">Your Instructions / Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">C1</t>
+    <t xml:space="preserve">C1, C2, C3, C5, C6, C7, C8, C9, C10, C12, C24, C101, C102, C104, C105, C107, C108, C109, C110, C111, C112, C201, C202, C204, C206, C208, C209, C300, C302</t>
   </si>
   <si>
     <t xml:space="preserve">KEMET</t>
   </si>
   <si>
-    <t xml:space="preserve">C1206C470K5GACTU </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP CER 47pf 50V X7R 1206</t>
+    <t xml:space="preserve">C1206C104K5RAC7800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 0.1UF 50V X7R 1206</t>
   </si>
   <si>
     <t xml:space="preserve">SMD</t>
   </si>
   <si>
-    <t xml:space="preserve">C2, C3, C4, C5, C9, C10, C12, C13, C14, C15, C17, C20, C21, C23, C25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1206C104K5RAC7867 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP CER 0.1UF 50V X7R 1206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C7, C8, C16, C19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1206C103K5RACTM </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP CER 0.01UF 50V X7R 1206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C18</t>
+    <t xml:space="preserve">L1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abracon LLC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIML-1206-R18K-T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIXED IND 180NH 250MA 300MOHM SM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L2, L101, L103, L201, L204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eaton - Electronics Division</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCLA3216V1-2R2-R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIXED IND 2.2UH 50MA 500MOHM SMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L102, L104, L202, L203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vishay / Dale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILSB1206ERR33K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIXED IND 330NH 250MA 600MOHM SMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R101, R103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE Connectivity Passive Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRG1206F100R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 100 OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R106, R107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stackpole Electronics Inc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMCF1206FT1K10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 1.1K OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R201, R204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRGCQ1206F56R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 56 OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R303</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMCF1206FT470R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 470 OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R306</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRG1206F220R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 220 OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C4</t>
   </si>
   <si>
     <t xml:space="preserve">Yageo</t>
   </si>
   <si>
-    <t xml:space="preserve">CC1206MRY5V9BB105 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP CER 1uF 50V Y5V 1206 20%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C6, C11</t>
+    <t xml:space="preserve">CC1206KRX7R9BB391</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 390PF 50V C0G/NP0 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C103, C106, C203, C207</t>
   </si>
   <si>
     <t xml:space="preserve">Samsung Electro-Mechanics</t>
   </si>
   <si>
-    <t xml:space="preserve">CL31A106KBHNNNE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP CER 10 UF 50V X7R 1206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EEV107M035A9HAA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alum CAP SMD 35V 100uF 20%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Infineon Technologies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IRLML9301TRPBF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOT-23-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comchip Technology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MMBT3904-HF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MMBT3904 SOT-23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R10, R11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC1206FR-075R1L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMD 5.1 Ohms 250 mW 1206 1%</t>
+    <t xml:space="preserve">CL31B474KBHNNNE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 0.47UF 50V X7R 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Würth Elektronik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 33PF 50V C0G/NP0 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C11, C301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chemi-Con</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMVE160ARA101MF55G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP ALUM 100UF 20% 16V 4.3X4.3 SMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.3x6.6mm</t>
   </si>
   <si>
     <t xml:space="preserve">R1</t>
   </si>
   <si>
-    <t xml:space="preserve">RC1206FR-076R8L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMD 6.8 Ohms 250 mW 1206 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R4, R5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEI Stackpole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RMCF1206FT100R </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMD 100 Ohms 250 mW 1206 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2, R3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vishay / Dale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRCW1206680RFKEAC </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMD 680 Ohms 250 mW 1206 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R12, R13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RMCF1206FT750R </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMD 750 Ohms 250 mW 1206 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R8, R9, R14, R15, R16, R17, R18, R19, R23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC1206FR-071KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMD 1000 Ohms 250 mW 1206 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R6, R7</t>
+    <t xml:space="preserve">RMCF1206FT4K70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 4.7K OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rohm Semiconductor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KTR18EZPF5101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 5.1K OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMCF1206FT200R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 200 OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4, R16, R304</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMCF1206FT150R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 150 OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMCF1206FT3K30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 3.3K OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMCF1206FT5K60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 5.6K OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7</t>
   </si>
   <si>
     <t xml:space="preserve">Bourns</t>
   </si>
   <si>
-    <t xml:space="preserve">CR1206-FX-2201ELF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMD 2.2K Ohms 250 mW 1206 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R22, R24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Welwyn Components / TT Electronics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WCR1206-10KFA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMD 10K Ohms 250 mW 1206 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Texas Instruments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPA2674ID </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPA2674ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOIC-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STMicroelectronics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L78L09ACUTR </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L78L09ACUTR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOT-89</t>
+    <t xml:space="preserve">CR1206-FX-1201ELF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 1.2K OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMCF1206JT68R0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 68 OHM 5% 1/4W 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMCF1206FT3K00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 3K OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMCF1206JT680R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 680 OHM 5% 1/4W 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R11, R13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMCF1206FT24K0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 24K OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R12, R15, R301, R302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMCF1206FT10K0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 10K OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMCF2512JT47R0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 47 OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KTR18EZPF37R4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 37.4 OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC1206FR-075K49L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 5.49K OHM 1% 1/4W 1206</t>
   </si>
   <si>
     <t xml:space="preserve">Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!</t>
@@ -631,9 +715,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>664560</xdr:colOff>
+      <xdr:colOff>665280</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>154800</xdr:rowOff>
+      <xdr:rowOff>155520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -647,7 +731,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="209520"/>
-          <a:ext cx="1455480" cy="374040"/>
+          <a:ext cx="1456200" cy="374760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -667,10 +751,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:I1048576"/>
+  <dimension ref="A2:I57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -737,7 +821,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="n">
         <v>1</v>
       </c>
@@ -745,7 +829,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>11</v>
@@ -764,7 +848,7 @@
       </c>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="n">
         <v>2</v>
       </c>
@@ -772,16 +856,16 @@
         <v>15</v>
       </c>
       <c r="C8" s="6" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G8" s="6" t="n">
         <v>1206</v>
@@ -791,24 +875,24 @@
       </c>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="n">
         <v>3</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G9" s="6" t="n">
         <v>1206</v>
@@ -818,24 +902,24 @@
       </c>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="n">
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G10" s="6" t="n">
         <v>1206</v>
@@ -850,19 +934,19 @@
         <v>5</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C11" s="6" t="n">
         <v>2</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G11" s="6" t="n">
         <v>1206</v>
@@ -877,49 +961,49 @@
         <v>6</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C12" s="6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="G12" s="6" t="n">
+        <v>1206</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="n">
         <v>7</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C13" s="6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="G13" s="6" t="n">
+        <v>1206</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>14</v>
@@ -931,13 +1015,13 @@
         <v>8</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>39</v>
@@ -945,15 +1029,15 @@
       <c r="F14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>36</v>
+      <c r="G14" s="6" t="n">
+        <v>1206</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="n">
         <v>9</v>
       </c>
@@ -961,10 +1045,10 @@
         <v>41</v>
       </c>
       <c r="C15" s="6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>42</v>
@@ -991,13 +1075,13 @@
         <v>1</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G16" s="6" t="n">
         <v>1206</v>
@@ -1007,24 +1091,24 @@
       </c>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="n">
         <v>11</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C17" s="6" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G17" s="6" t="n">
         <v>1206</v>
@@ -1039,16 +1123,16 @@
         <v>12</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C18" s="6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="6" t="s">
         <v>53</v>
+      </c>
+      <c r="E18" s="6" t="n">
+        <v>885012008040</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>54</v>
@@ -1072,40 +1156,40 @@
         <v>2</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="6" t="n">
-        <v>1206</v>
+        <v>58</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="n">
         <v>14</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C20" s="6" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G20" s="6" t="n">
         <v>1206</v>
@@ -1120,19 +1204,19 @@
         <v>15</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C21" s="6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G21" s="6" t="n">
         <v>1206</v>
@@ -1142,24 +1226,24 @@
       </c>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="n">
         <v>16</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C22" s="6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>1206</v>
@@ -1174,13 +1258,13 @@
         <v>17</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C23" s="6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>71</v>
@@ -1188,8 +1272,8 @@
       <c r="F23" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="G23" s="6" t="s">
-        <v>73</v>
+      <c r="G23" s="6" t="n">
+        <v>1206</v>
       </c>
       <c r="H23" s="6" t="s">
         <v>14</v>
@@ -1201,136 +1285,296 @@
         <v>18</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C24" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D24" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="G24" s="6" t="n">
+        <v>1206</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="C25" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="F25" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="H24" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I24" s="7"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
+      <c r="G25" s="6" t="n">
+        <v>1206</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G26" s="6" t="n">
+        <v>1206</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="I26" s="7"/>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="n">
+        <v>21</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27" s="6" t="n">
+        <v>1206</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="n">
+        <v>22</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" s="6" t="n">
+        <v>1206</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="I28" s="7"/>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G29" s="6" t="n">
+        <v>1206</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="I29" s="7"/>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
+    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G30" s="6" t="n">
+        <v>1206</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
+    <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G31" s="6" t="n">
+        <v>1206</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
+    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="n">
+        <v>26</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G32" s="6" t="n">
+        <v>1206</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
+    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="n">
+        <v>27</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="G33" s="6" t="n">
+        <v>1206</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="I33" s="7"/>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
+    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="n">
+        <v>28</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G34" s="6" t="n">
+        <v>1206</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="I34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1342,7 +1586,7 @@
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
-      <c r="I35" s="8"/>
+      <c r="I35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6"/>
@@ -1353,7 +1597,7 @@
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
-      <c r="I36" s="7"/>
+      <c r="I36" s="8"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6"/>
@@ -1430,7 +1674,7 @@
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
-      <c r="I43" s="8"/>
+      <c r="I43" s="7"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6"/>
@@ -1441,7 +1685,7 @@
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
-      <c r="I44" s="7"/>
+      <c r="I44" s="8"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6"/>
@@ -1496,6 +1740,7 @@
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
+      <c r="I49" s="7"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="6"/>
@@ -1517,56 +1762,65 @@
       <c r="G51" s="6"/>
       <c r="H51" s="6"/>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="6"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+    </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="B54" s="9"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
-    </row>
-    <row r="55" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="10"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="10"/>
-      <c r="G55" s="10"/>
-      <c r="H55" s="10"/>
-      <c r="I55" s="10"/>
-    </row>
-    <row r="56" s="12" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B56" s="11"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
-      <c r="I56" s="11"/>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="10"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
+    </row>
+    <row r="57" s="12" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="D2:F4"/>
-    <mergeCell ref="A54:I54"/>
-    <mergeCell ref="A56:I56"/>
+    <mergeCell ref="A55:I55"/>
+    <mergeCell ref="A57:I57"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A54" r:id="rId1" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!"/>
-    <hyperlink ref="A56" r:id="rId2" display="Click for Instructions on How to Create a BOM"/>
+    <hyperlink ref="A55" r:id="rId1" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!"/>
+    <hyperlink ref="A57" r:id="rId2" display="Click for Instructions on How to Create a BOM"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>